<commit_message>
plots per patients added
</commit_message>
<xml_diff>
--- a/gegevens groeisnelheid - Copy 29-4 naar Bart.xlsx
+++ b/gegevens groeisnelheid - Copy 29-4 naar Bart.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="25440" windowHeight="12375" firstSheet="33" activeTab="45"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="25440" windowHeight="12375" firstSheet="36" activeTab="48"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -8346,7 +8346,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -8811,8 +8811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8872,7 +8872,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>74</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -9300,8 +9300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>